<commit_message>
fix(module3): use uncon_planned_qty for future production; keep produced for today
- 修复读取future production plan为空的问题
- 修复使用begining inventory计算available inventory
</commit_message>
<xml_diff>
--- a/e2e_test_output_12week_forecast_test/simulation_output/module1/module1_output_20240103.xlsx
+++ b/e2e_test_output_12week_forecast_test/simulation_output/module1/module1_output_20240103.xlsx
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>45294</v>
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>45294</v>
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>45294</v>
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>45294</v>
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1033,7 +1033,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>

</xml_diff>